<commit_message>
Homepage Registration and exlsdata modified
</commit_message>
<xml_diff>
--- a/src/main/java/com_Embrio_TestData/Embriodata.xlsx
+++ b/src/main/java/com_Embrio_TestData/Embriodata.xlsx
@@ -12,23 +12,24 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
-    <sheet name="HomePage" sheetId="1" r:id="rId2"/>
-    <sheet name="EMRPage" sheetId="7" r:id="rId3"/>
-    <sheet name="Addictions" sheetId="6" r:id="rId4"/>
-    <sheet name="Vitals" sheetId="2" r:id="rId5"/>
-    <sheet name="Complaints" sheetId="13" r:id="rId6"/>
-    <sheet name="SexualHistory" sheetId="3" r:id="rId7"/>
-    <sheet name="pastMedicationHistory" sheetId="4" r:id="rId8"/>
-    <sheet name="Investigation" sheetId="8" r:id="rId9"/>
-    <sheet name="CycleList" sheetId="11" r:id="rId10"/>
-    <sheet name="Stimulationchart" sheetId="14" r:id="rId11"/>
-    <sheet name="Diagnosis" sheetId="12" r:id="rId12"/>
-    <sheet name="InvestigationList" sheetId="9" r:id="rId13"/>
-    <sheet name="Family History" sheetId="16" r:id="rId14"/>
-    <sheet name="OverviewPage" sheetId="17" r:id="rId15"/>
-    <sheet name="Allergies" sheetId="10" r:id="rId16"/>
-    <sheet name="ObstetricHistory" sheetId="18" r:id="rId17"/>
+    <sheet name="Name" sheetId="19" r:id="rId1"/>
+    <sheet name="LoginPage" sheetId="5" r:id="rId2"/>
+    <sheet name="HomePage" sheetId="1" r:id="rId3"/>
+    <sheet name="EMRPage" sheetId="7" r:id="rId4"/>
+    <sheet name="Addictions" sheetId="6" r:id="rId5"/>
+    <sheet name="Vitals" sheetId="2" r:id="rId6"/>
+    <sheet name="Complaints" sheetId="13" r:id="rId7"/>
+    <sheet name="SexualHistory" sheetId="3" r:id="rId8"/>
+    <sheet name="pastMedicationHistory" sheetId="4" r:id="rId9"/>
+    <sheet name="Investigation" sheetId="8" r:id="rId10"/>
+    <sheet name="CycleList" sheetId="11" r:id="rId11"/>
+    <sheet name="Stimulationchart" sheetId="14" r:id="rId12"/>
+    <sheet name="Diagnosis" sheetId="12" r:id="rId13"/>
+    <sheet name="InvestigationList" sheetId="9" r:id="rId14"/>
+    <sheet name="Family History" sheetId="16" r:id="rId15"/>
+    <sheet name="OverviewPage" sheetId="17" r:id="rId16"/>
+    <sheet name="Allergies" sheetId="10" r:id="rId17"/>
+    <sheet name="ObstetricHistory" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="ERLinked">Investigation!$I$2:$I$3</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2005" uniqueCount="1119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="1143">
   <si>
     <t>PatientName</t>
   </si>
@@ -3408,6 +3409,78 @@
   </si>
   <si>
     <t>Anuradha.A</t>
+  </si>
+  <si>
+    <t>PatientLastName</t>
+  </si>
+  <si>
+    <t>PatientDOBYear</t>
+  </si>
+  <si>
+    <t>PatientDOBMonth</t>
+  </si>
+  <si>
+    <t>PatientDOBDay</t>
+  </si>
+  <si>
+    <t>PatientFirstName</t>
+  </si>
+  <si>
+    <t>PatientMiddleName</t>
+  </si>
+  <si>
+    <t>PartnerFirstName</t>
+  </si>
+  <si>
+    <t>PartnerMiddleName</t>
+  </si>
+  <si>
+    <t>PartnerLastName</t>
+  </si>
+  <si>
+    <t>PartnerDOBYear</t>
+  </si>
+  <si>
+    <t>PartnerDOBMonth</t>
+  </si>
+  <si>
+    <t>PartnerDOBDay</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Ganesh</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>Suresh</t>
+  </si>
+  <si>
+    <t>Ritesh</t>
+  </si>
+  <si>
+    <t>Himesh</t>
+  </si>
+  <si>
+    <t>Jignesh</t>
+  </si>
+  <si>
+    <t>Kalpesh</t>
+  </si>
+  <si>
+    <t>Rupesh</t>
+  </si>
+  <si>
+    <t>Dhanesh</t>
+  </si>
+  <si>
+    <t>Nilesh</t>
   </si>
 </sst>
 </file>
@@ -3807,56 +3880,736 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1">
+    <row r="1" spans="1:12">
+      <c r="A1" s="17" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>1120</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>1121</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>1122</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>1128</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>1129</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G2">
+        <v>1980</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>1975</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G3">
+        <v>1981</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <v>1976</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G4">
+        <v>1982</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>1977</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G5">
+        <v>1983</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <v>1978</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G6">
+        <v>1984</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>1979</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G7">
+        <v>1985</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>1980</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G8">
+        <v>1986</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <v>1981</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G9">
+        <v>1987</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>17</v>
+      </c>
+      <c r="J9">
+        <v>1982</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G10">
+        <v>1988</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <v>1983</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+      <c r="L10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G11">
+        <v>1989</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>19</v>
+      </c>
+      <c r="J11">
+        <v>1984</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G12">
+        <v>1990</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>1985</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G13">
+        <v>1991</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>21</v>
+      </c>
+      <c r="J13">
+        <v>1986</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G14">
+        <v>1992</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>22</v>
+      </c>
+      <c r="J14">
+        <v>1987</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="10" customFormat="1">
       <c r="A1" s="7" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>131</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>1118</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="L2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="B3" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>118</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="L9" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="L10" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="L11" t="s">
+        <v>1047</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+      <formula1>"package+$A$10"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1502"/>
   <sheetViews>
@@ -3960,7 +4713,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43305</v>
+        <v>43306</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11673,7 +12426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E116"/>
   <sheetViews>
@@ -11718,11 +12471,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43305</v>
+        <v>43306</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43305</v>
+        <v>43306</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12337,7 +13090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -12380,7 +13133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -12476,7 +13229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -12582,7 +13335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -12611,7 +13364,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:E3"/>
   <sheetViews>
@@ -12648,7 +13401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -12673,6 +13426,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="10" customFormat="1">
+      <c r="A1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C55"/>
@@ -13107,7 +13911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:A4"/>
@@ -13145,7 +13949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H6"/>
@@ -13307,7 +14111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G6"/>
@@ -13468,7 +14272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -13502,7 +14306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O27"/>
@@ -14050,7 +14854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G13"/>
@@ -14134,217 +14938,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:L11"/>
-  <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1">
-      <c r="A1" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" t="s">
-        <v>120</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1042</v>
-      </c>
-      <c r="L2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="B3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" t="s">
-        <v>133</v>
-      </c>
-      <c r="L3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="B4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H4" t="s">
-        <v>126</v>
-      </c>
-      <c r="L4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="B5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" t="s">
-        <v>137</v>
-      </c>
-      <c r="H5" t="s">
-        <v>127</v>
-      </c>
-      <c r="L5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="B6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" t="s">
-        <v>121</v>
-      </c>
-      <c r="L6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="B7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C7" t="s">
-        <v>122</v>
-      </c>
-      <c r="L7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="B8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" t="s">
-        <v>123</v>
-      </c>
-      <c r="L8" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="L9" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="L10" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="L11" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
-      <formula1>"package+$A$10"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Addedscreenshotmethod inutil class and modified TestNGListners
</commit_message>
<xml_diff>
--- a/src/main/java/com_Embrio_TestData/Embriodata.xlsx
+++ b/src/main/java/com_Embrio_TestData/Embriodata.xlsx
@@ -9,27 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Name" sheetId="19" r:id="rId1"/>
     <sheet name="LoginPage" sheetId="5" r:id="rId2"/>
-    <sheet name="HomePage" sheetId="1" r:id="rId3"/>
-    <sheet name="EMRPage" sheetId="7" r:id="rId4"/>
-    <sheet name="Addictions" sheetId="6" r:id="rId5"/>
-    <sheet name="Vitals" sheetId="2" r:id="rId6"/>
-    <sheet name="Complaints" sheetId="13" r:id="rId7"/>
-    <sheet name="SexualHistory" sheetId="3" r:id="rId8"/>
-    <sheet name="pastMedicationHistory" sheetId="4" r:id="rId9"/>
-    <sheet name="Investigation" sheetId="8" r:id="rId10"/>
-    <sheet name="CycleList" sheetId="11" r:id="rId11"/>
-    <sheet name="Stimulationchart" sheetId="14" r:id="rId12"/>
-    <sheet name="Diagnosis" sheetId="12" r:id="rId13"/>
-    <sheet name="InvestigationList" sheetId="9" r:id="rId14"/>
-    <sheet name="Family History" sheetId="16" r:id="rId15"/>
-    <sheet name="OverviewPage" sheetId="17" r:id="rId16"/>
-    <sheet name="Allergies" sheetId="10" r:id="rId17"/>
-    <sheet name="ObstetricHistory" sheetId="18" r:id="rId18"/>
+    <sheet name="RegistrationPage" sheetId="20" r:id="rId3"/>
+    <sheet name="HomePage" sheetId="1" r:id="rId4"/>
+    <sheet name="EMRPage" sheetId="7" r:id="rId5"/>
+    <sheet name="Addictions" sheetId="6" r:id="rId6"/>
+    <sheet name="Vitals" sheetId="2" r:id="rId7"/>
+    <sheet name="Complaints" sheetId="13" r:id="rId8"/>
+    <sheet name="SexualHistory" sheetId="3" r:id="rId9"/>
+    <sheet name="pastMedicationHistory" sheetId="4" r:id="rId10"/>
+    <sheet name="Investigation" sheetId="8" r:id="rId11"/>
+    <sheet name="CycleList" sheetId="11" r:id="rId12"/>
+    <sheet name="Stimulationchart" sheetId="14" r:id="rId13"/>
+    <sheet name="Diagnosis" sheetId="12" r:id="rId14"/>
+    <sheet name="InvestigationList" sheetId="9" r:id="rId15"/>
+    <sheet name="Family History" sheetId="16" r:id="rId16"/>
+    <sheet name="OverviewPage" sheetId="17" r:id="rId17"/>
+    <sheet name="Allergies" sheetId="10" r:id="rId18"/>
+    <sheet name="ObstetricHistory" sheetId="18" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="ERLinked">Investigation!$I$2:$I$3</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="1177">
   <si>
     <t>PatientName</t>
   </si>
@@ -3481,6 +3482,108 @@
   </si>
   <si>
     <t>Nilesh</t>
+  </si>
+  <si>
+    <t>Fill all mandatory fields.</t>
+  </si>
+  <si>
+    <t>1980</t>
+  </si>
+  <si>
+    <t>1981</t>
+  </si>
+  <si>
+    <t>1982</t>
+  </si>
+  <si>
+    <t>1983</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>1985</t>
+  </si>
+  <si>
+    <t>1986</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>1975</t>
+  </si>
+  <si>
+    <t>1976</t>
+  </si>
+  <si>
+    <t>1977</t>
+  </si>
+  <si>
+    <t>1978</t>
+  </si>
+  <si>
+    <t>1979</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>MobileNoPatient</t>
+  </si>
+  <si>
+    <t>MobileNoPartner</t>
   </si>
 </sst>
 </file>
@@ -3882,8 +3985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4397,6 +4500,92 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="10" customFormat="1">
+      <c r="A1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1">
+      <c r="A2" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:L11"/>
@@ -4609,7 +4798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1502"/>
   <sheetViews>
@@ -4713,7 +4902,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43306</v>
+        <v>43315</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -12426,7 +12615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E116"/>
   <sheetViews>
@@ -12471,11 +12660,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43306</v>
+        <v>43315</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43306</v>
+        <v>43315</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -13090,7 +13279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -13133,7 +13322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -13229,7 +13418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -13335,7 +13524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -13364,7 +13553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:E3"/>
   <sheetViews>
@@ -13401,7 +13590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -13478,6 +13667,587 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>1122</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>1128</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>1129</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>1130</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>1175</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>1162</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>1156</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>1162</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2">
+        <v>9856321587</v>
+      </c>
+      <c r="O2">
+        <v>9523159870</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>1145</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>1163</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>1157</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>1163</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="N3">
+        <v>9856321588</v>
+      </c>
+      <c r="O3">
+        <v>9523159871</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="B4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>1146</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>1164</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>1158</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>1164</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4">
+        <v>9856321589</v>
+      </c>
+      <c r="O4">
+        <v>9523159872</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1136</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>1147</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>1165</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>1159</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>1165</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N5">
+        <v>9856321590</v>
+      </c>
+      <c r="O5">
+        <v>9523159873</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>1148</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>1166</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>1160</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>1166</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N6">
+        <v>9856321591</v>
+      </c>
+      <c r="O6">
+        <v>9523159874</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1138</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>1149</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>1167</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>1167</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7">
+        <v>9856321592</v>
+      </c>
+      <c r="O7">
+        <v>9523159875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1139</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>1150</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>1168</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>1174</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>1145</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>1168</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>1174</v>
+      </c>
+      <c r="N8">
+        <v>9856321593</v>
+      </c>
+      <c r="O8">
+        <v>9523159876</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="B9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>1169</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>1042</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>1146</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>1169</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>1042</v>
+      </c>
+      <c r="N9">
+        <v>9856321594</v>
+      </c>
+      <c r="O9">
+        <v>9523159877</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="B10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1141</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>1152</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>1170</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>1147</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>1170</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="N10">
+        <v>9856321595</v>
+      </c>
+      <c r="O10">
+        <v>9523159878</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>1153</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>1148</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>1171</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="N11">
+        <v>9856321596</v>
+      </c>
+      <c r="O11">
+        <v>9523159879</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="B12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>1154</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>1172</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>1149</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>1172</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="N12">
+        <v>9856321597</v>
+      </c>
+      <c r="O12">
+        <v>9523159880</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="B13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1136</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>1155</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>1173</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>1161</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>1150</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>1173</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>1161</v>
+      </c>
+      <c r="N13">
+        <v>9856321598</v>
+      </c>
+      <c r="O13">
+        <v>9523159881</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C55"/>
   <sheetViews>
@@ -13911,7 +14681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:A4"/>
@@ -13949,7 +14719,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H6"/>
@@ -14111,7 +14881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G6"/>
@@ -14272,7 +15042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -14306,7 +15076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O27"/>
@@ -14852,90 +15622,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:G13"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1">
-      <c r="A1" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="10" customFormat="1">
-      <c r="A2" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>